<commit_message>
rerun with new data
</commit_message>
<xml_diff>
--- a/data/HBGDki-tab1-shell.xlsx
+++ b/data/HBGDki-tab1-shell.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\HBGDki\ki-longitudinal-manuscripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4A41DF4-1691-4D0D-AFA4-1847B4011CE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4360562C-CB65-4FDC-B99C-3C54D1C4249D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9114" yWindow="0" windowWidth="13902" windowHeight="12210"/>
+    <workbookView xWindow="11328" yWindow="936" windowWidth="11106" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HBGDki-tab1-shell" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -571,7 +579,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1656,10 +1664,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -3106,38 +3116,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/EE?preview=Promising_Biomarkers_of_Environmental_Enteric_Dysf.pdf"/>
-    <hyperlink ref="H4" r:id="rId2" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Respak?preview=Ali_et_al-2016-Journal_of_Medical_Virology.pdf"/>
-    <hyperlink ref="H6" r:id="rId3" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Shrestha+et+al+2014+Clin+Infect+Dis+NPL.pdf"/>
-    <hyperlink ref="H7" r:id="rId4" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/CMC-V-BCS-2002 (Vellore Rotavirus)?preview=Sarkar+et+al+2013+PlosOne.PDF"/>
-    <hyperlink ref="H8" r:id="rId5" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=John+et+al+2014+Clin+Infect+Dis+IND.pdf"/>
-    <hyperlink ref="H9" r:id="rId6" display="https://www.dropbox.com/preview/HBGDki documentation/ghap study doc folders/TDC (Vellore Bottled Water)/Sarkar et al. 2013 BMC Public Health.pdf?role=personal"/>
-    <hyperlink ref="H10" r:id="rId7" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/CMIN/Bangladesh?preview=Pathela+et+al+2006+Acta+Paediatrica.pdf"/>
-    <hyperlink ref="H11" r:id="rId8" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Ahmed+et+al+2014+Clin+Infect+Dis.pdf"/>
-    <hyperlink ref="H12" r:id="rId9" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Provide?preview=Kirkpatrick+et+al+2015+Am+J+Trop+Med+Hyg.pdf"/>
-    <hyperlink ref="H13" r:id="rId10" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/SAS-FoodSuppl?preview=Bhandari+et+al+2001+J+Nutri.pdf"/>
-    <hyperlink ref="H14" r:id="rId11" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/SAS-compfeeding?preview=Bhandari+et+al+2004+J+Nutri.pdf"/>
-    <hyperlink ref="H15" r:id="rId12" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/India?preview=Bhargava+et+al+2009+NEJM.pdf"/>
-    <hyperlink ref="H17" r:id="rId13" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Jivita-4?preview=Christian+2015+IJE+.pdf"/>
-    <hyperlink ref="H18" r:id="rId14" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Jivita 3?preview=Christian+et+al+2016+AJCN.pdf"/>
-    <hyperlink ref="H19" r:id="rId15" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/NIH-Crypto?preview=Steiner+et+al+2018+Clin+Infect+Dis.pdf"/>
-    <hyperlink ref="H20" r:id="rId16" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/Philippines?preview=Adair+2007+Am+J+Hum+Biol.pdf"/>
-    <hyperlink ref="H22" r:id="rId17" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Mduma+et+al+2014+Clin+Infect+Dis+TZN.pdf"/>
-    <hyperlink ref="H23" r:id="rId18" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Tanzania Child 2?preview=Locks+et+al+Am+J+Clin+Nutr+2016.pdf"/>
-    <hyperlink ref="H24" r:id="rId19" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Bessong+et+al+2014+Clin+Infect+Dis+SA.pdf"/>
-    <hyperlink ref="H26" r:id="rId20" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/ZVitambo?preview=Malaba+2005+Am+J+Clin+Nutr.pdf"/>
-    <hyperlink ref="H27" r:id="rId21" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dyad-M?preview=Ashorn+et+al+2015+J.+Nutr.pdf"/>
-    <hyperlink ref="H28" r:id="rId22" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Zinc?preview=Hess+et+al+2015+PlosOne.PDF"/>
-    <hyperlink ref="H30" r:id="rId23" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Yori+et+al+2014+Clin+Infect+Dis+PER.pdf"/>
-    <hyperlink ref="H31" r:id="rId24" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/CONTENT?preview=Jaganath+et+al+2014+Helicobacter.pdf"/>
-    <hyperlink ref="H32" r:id="rId25" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Guatemala BSC/docs?preview=Begin+bovine+serum+micronut+growth+Guat+EJCN2008.pdf"/>
-    <hyperlink ref="H33" r:id="rId26" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/mal-ed?preview=Lima+et+al+2014+Clin+Infect+Dis.pdf"/>
-    <hyperlink ref="H34" r:id="rId27" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/Guatemala?preview=Habicht+et+al+1995+J+Nutr.pdf"/>
-    <hyperlink ref="H36" r:id="rId28" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/PROBIT?preview=Kramer+et+al+2001+JAMA.pdf"/>
-    <hyperlink ref="H38" r:id="rId29" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Burkina Faso Zn?preview=Becquey+et+al+2016+J+Nutr.pdf"/>
-    <hyperlink ref="H39" r:id="rId30" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Vitamin-A?preview=WHO+CHD+Vitamin+A+Group+1998+Lancet.pdf"/>
-    <hyperlink ref="H40" r:id="rId31" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dose?preview=Phuka+et+al+2008+Arch+Pediatr+Adolesc+Med.pdf"/>
-    <hyperlink ref="H41" r:id="rId32" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dyad-M?preview=Ashorn+et+al+2015+J.+Nutr.pdf"/>
+    <hyperlink ref="H3" r:id="rId1" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/EE?preview=Promising_Biomarkers_of_Environmental_Enteric_Dysf.pdf" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H4" r:id="rId2" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Respak?preview=Ali_et_al-2016-Journal_of_Medical_Virology.pdf" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H6" r:id="rId3" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Shrestha+et+al+2014+Clin+Infect+Dis+NPL.pdf" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/CMC-V-BCS-2002 (Vellore Rotavirus)?preview=Sarkar+et+al+2013+PlosOne.PDF" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H8" r:id="rId5" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=John+et+al+2014+Clin+Infect+Dis+IND.pdf" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H9" r:id="rId6" display="https://www.dropbox.com/preview/HBGDki documentation/ghap study doc folders/TDC (Vellore Bottled Water)/Sarkar et al. 2013 BMC Public Health.pdf?role=personal" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H10" r:id="rId7" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/CMIN/Bangladesh?preview=Pathela+et+al+2006+Acta+Paediatrica.pdf" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H11" r:id="rId8" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Ahmed+et+al+2014+Clin+Infect+Dis.pdf" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H12" r:id="rId9" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Provide?preview=Kirkpatrick+et+al+2015+Am+J+Trop+Med+Hyg.pdf" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H13" r:id="rId10" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/SAS-FoodSuppl?preview=Bhandari+et+al+2001+J+Nutri.pdf" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/SAS-compfeeding?preview=Bhandari+et+al+2004+J+Nutri.pdf" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H15" r:id="rId12" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/India?preview=Bhargava+et+al+2009+NEJM.pdf" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H17" r:id="rId13" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Jivita-4?preview=Christian+2015+IJE+.pdf" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H18" r:id="rId14" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Jivita 3?preview=Christian+et+al+2016+AJCN.pdf" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H19" r:id="rId15" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/NIH-Crypto?preview=Steiner+et+al+2018+Clin+Infect+Dis.pdf" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H20" r:id="rId16" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/Philippines?preview=Adair+2007+Am+J+Hum+Biol.pdf" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H22" r:id="rId17" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Mduma+et+al+2014+Clin+Infect+Dis+TZN.pdf" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H23" r:id="rId18" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Tanzania Child 2?preview=Locks+et+al+Am+J+Clin+Nutr+2016.pdf" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H24" r:id="rId19" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Bessong+et+al+2014+Clin+Infect+Dis+SA.pdf" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H26" r:id="rId20" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/ZVitambo?preview=Malaba+2005+Am+J+Clin+Nutr.pdf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H27" r:id="rId21" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dyad-M?preview=Ashorn+et+al+2015+J.+Nutr.pdf" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H28" r:id="rId22" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Zinc?preview=Hess+et+al+2015+PlosOne.PDF" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H30" r:id="rId23" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/mal-ed?preview=Yori+et+al+2014+Clin+Infect+Dis+PER.pdf" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H31" r:id="rId24" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/CONTENT?preview=Jaganath+et+al+2014+Helicobacter.pdf" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H32" r:id="rId25" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/Guatemala BSC/docs?preview=Begin+bovine+serum+micronut+growth+Guat+EJCN2008.pdf" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H33" r:id="rId26" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/mal-ed?preview=Lima+et+al+2014+Clin+Infect+Dis.pdf" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H34" r:id="rId27" display="https://www.dropbox.com/home/HBGDki documentation/ghap study doc folders/COHORTS/Guatemala?preview=Habicht+et+al+1995+J+Nutr.pdf" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H36" r:id="rId28" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/PROBIT?preview=Kramer+et+al+2001+JAMA.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H38" r:id="rId29" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Burkina Faso Zn?preview=Becquey+et+al+2016+J+Nutr.pdf" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H39" r:id="rId30" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/Vitamin-A?preview=WHO+CHD+Vitamin+A+Group+1998+Lancet.pdf" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H40" r:id="rId31" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dose?preview=Phuka+et+al+2008+Arch+Pediatr+Adolesc+Med.pdf" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H41" r:id="rId32" display="https://www.dropbox.com/home/HBGDki documentation/GHAP Study Doc folders/iLiNS-Dyad-M?preview=Ashorn+et+al+2015+J.+Nutr.pdf" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>

</xml_diff>